<commit_message>
v0.0.2 - gcp deply and versioning
</commit_message>
<xml_diff>
--- a/resumefit/pm/resumefit-tracker.xlsx
+++ b/resumefit/pm/resumefit-tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\vivek\projects\resumefit\pm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68808F7C-5B20-4463-93D8-598FB28DE11C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186D8D9A-0FEB-436B-92C8-FA5279466ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-8865" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
   <si>
     <t>version</t>
   </si>
@@ -75,6 +75,9 @@
     <t>0.0.2</t>
   </si>
   <si>
+    <t>0.0.3</t>
+  </si>
+  <si>
     <t>implemented</t>
   </si>
   <si>
@@ -141,13 +144,22 @@
     <t>provide user sections to craft their resume</t>
   </si>
   <si>
-    <t>versioning of the api server and web server</t>
-  </si>
-  <si>
     <t>preparation for the company - about the company and its customers</t>
   </si>
   <si>
     <t>top 10 questions you may be asekd with answers</t>
+  </si>
+  <si>
+    <t>provide alternatives for gpt-4o to gemini</t>
+  </si>
+  <si>
+    <t>handle pdf creation in the backend</t>
+  </si>
+  <si>
+    <t>versioning of the api server</t>
+  </si>
+  <si>
+    <t>version in web app</t>
   </si>
 </sst>
 </file>
@@ -469,7 +481,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,13 +501,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -603,10 +615,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -617,7 +629,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -637,7 +649,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -657,10 +669,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
         <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
       </c>
       <c r="D10">
         <v>2</v>
@@ -671,24 +683,28 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
         <v>20</v>
-      </c>
-      <c r="C12" t="s">
-        <v>19</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -699,13 +715,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D13">
         <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="1">
+        <v>45577</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -713,10 +735,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -727,13 +749,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
       </c>
       <c r="D15">
         <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="1">
+        <v>45576</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -744,13 +772,13 @@
         <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -758,43 +786,76 @@
         <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="1">
+        <v>45577</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -820,59 +881,59 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v0.0.3-limit characters, add download endpoint, versioning, cookie tracking, release notes
</commit_message>
<xml_diff>
--- a/resumefit/pm/resumefit-tracker.xlsx
+++ b/resumefit/pm/resumefit-tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\vivek\projects\resumefit\pm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186D8D9A-0FEB-436B-92C8-FA5279466ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E308F1-5A87-4547-8CF6-0B17E1631A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-8865" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22305" yWindow="-5235" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="features" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="44">
   <si>
     <t>version</t>
   </si>
@@ -147,9 +147,6 @@
     <t>preparation for the company - about the company and its customers</t>
   </si>
   <si>
-    <t>top 10 questions you may be asekd with answers</t>
-  </si>
-  <si>
     <t>provide alternatives for gpt-4o to gemini</t>
   </si>
   <si>
@@ -160,6 +157,18 @@
   </si>
   <si>
     <t>version in web app</t>
+  </si>
+  <si>
+    <t>resolve domain redirect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add release notes to keep track </t>
+  </si>
+  <si>
+    <t>tab icon update from vue</t>
+  </si>
+  <si>
+    <t>top 10 questions you may be asked with answers</t>
   </si>
 </sst>
 </file>
@@ -478,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,7 +703,9 @@
       <c r="E11" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="1">
+        <v>45577</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -709,6 +720,12 @@
       <c r="D12">
         <v>1</v>
       </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="1">
+        <v>45577</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -749,7 +766,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
@@ -783,7 +800,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
@@ -797,7 +814,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
@@ -811,13 +828,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
         <v>9</v>
       </c>
       <c r="D19">
         <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="1">
+        <v>45577</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -825,7 +848,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
@@ -844,24 +867,74 @@
       <c r="A21">
         <v>20</v>
       </c>
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="1">
+        <v>45577</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="1">
+        <v>45577</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
     </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>